<commit_message>
Initial upload of Excel Projects for DATA ANALYSIS
</commit_message>
<xml_diff>
--- a/Project2_PivotTables_Sales.xlsx
+++ b/Project2_PivotTables_Sales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Env't\Video_Tution\Udemy\Data_Analysis\Excel_Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F85AF71-C210-4C73-AED0-2624C60BB3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DB630F-3E27-4A99-9710-A94786BAA04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23985" windowHeight="14280" tabRatio="743" xr2:uid="{F7EB8B45-8F93-4DDF-81FD-2951E9FFEE63}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="743" activeTab="1" xr2:uid="{F7EB8B45-8F93-4DDF-81FD-2951E9FFEE63}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -68,7 +68,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId12"/>
+    <pivotCache cacheId="16" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -8644,7 +8644,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Dashboard!$A$1:$V$29" spid="_x0000_s15414"/>
+                  <a14:cameraTool cellRange="Dashboard!$A$1:$V$29" spid="_x0000_s15415"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -16526,7 +16526,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CB4186BE-B3A4-45EB-80D3-6C4FA307C0EC}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CB4186BE-B3A4-45EB-80D3-6C4FA307C0EC}" name="PivotTable1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
   <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -16678,7 +16678,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{688E8890-354D-4F8E-879B-805C2689FCD5}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="20">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{688E8890-354D-4F8E-879B-805C2689FCD5}" name="PivotTable1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="20">
   <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0" sortType="ascending">
@@ -16833,7 +16833,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CD9BDC1D-D8BA-4B0F-8E79-66AFD01013F8}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="29">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CD9BDC1D-D8BA-4B0F-8E79-66AFD01013F8}" name="PivotTable1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="29">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0" sortType="ascending">
@@ -17021,7 +17021,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{46D8D161-75F7-4DEB-A1EF-F65CD22BE8F5}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="30">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{46D8D161-75F7-4DEB-A1EF-F65CD22BE8F5}" name="PivotTable1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="30">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0" sortType="ascending">
@@ -17191,7 +17191,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{777653AE-F4C1-4405-AE5D-8E6EF42D947E}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="35">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{777653AE-F4C1-4405-AE5D-8E6EF42D947E}" name="PivotTable1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="35">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0" sortType="ascending">
@@ -17334,7 +17334,117 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B49B94E3-4613-4AC0-93CD-44AC4D42FF58}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ECB61868-E8AA-48E1-BE63-8C32BA9530EE}" name="PivotTable4" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E3:F8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="1"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="15" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="3" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Customer" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <filters count="1">
+    <filter fld="4" type="dateBetween" evalOrder="-1" id="333" name="Date">
+      <autoFilter ref="A1">
+        <filterColumn colId="0">
+          <customFilters and="1">
+            <customFilter operator="greaterThanOrEqual" val="43831"/>
+            <customFilter operator="lessThanOrEqual" val="44196"/>
+          </customFilters>
+        </filterColumn>
+      </autoFilter>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{0605FD5F-26C8-4aeb-8148-2DB25E43C511}">
+          <x15:pivotFilter useWholeDay="1"/>
+        </ext>
+      </extLst>
+    </filter>
+  </filters>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B49B94E3-4613-4AC0-93CD-44AC4D42FF58}" name="PivotTable3" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -17437,8 +17547,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E01F7F72-C2E9-4DC6-8C33-CFD9AF5BE672}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E01F7F72-C2E9-4DC6-8C33-CFD9AF5BE672}" name="PivotTable5" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="K3:L8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -17494,116 +17604,6 @@
   </pivotFields>
   <rowFields count="1">
     <field x="1"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Customer" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <filters count="1">
-    <filter fld="4" type="dateBetween" evalOrder="-1" id="333" name="Date">
-      <autoFilter ref="A1">
-        <filterColumn colId="0">
-          <customFilters and="1">
-            <customFilter operator="greaterThanOrEqual" val="43831"/>
-            <customFilter operator="lessThanOrEqual" val="44196"/>
-          </customFilters>
-        </filterColumn>
-      </autoFilter>
-      <extLst>
-        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{0605FD5F-26C8-4aeb-8148-2DB25E43C511}">
-          <x15:pivotFilter useWholeDay="1"/>
-        </ext>
-      </extLst>
-    </filter>
-  </filters>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ECB61868-E8AA-48E1-BE63-8C32BA9530EE}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E3:F8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="6">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="1"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="6">
-        <item x="4"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="15" showAll="0">
-      <items count="15">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="3" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
   </rowFields>
   <rowItems count="5">
     <i>
@@ -18036,7 +18036,7 @@
   </sheetPr>
   <dimension ref="A1:W31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A17" workbookViewId="0">
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
@@ -18185,7 +18185,7 @@
   </sheetPr>
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="94" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="94" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>